<commit_message>
Vietsub giao diện + Api checkout + chức năng checkout + thanh toán online VNpay + thêm chức năng gửi email có kèm file + fix search (bao gồm gợi ý autocomplete) + thêm option khách hàng ko login vẫn mua hàng + chỉnh lại store
</commit_message>
<xml_diff>
--- a/Kinh_Doanh_Khoa_Hoc_Truc_Tuyen_Api/wwwroot/attachments/form/Hoa_Don_Ban_Hang_Le.xlsx
+++ b/Kinh_Doanh_Khoa_Hoc_Truc_Tuyen_Api/wwwroot/attachments/form/Hoa_Don_Ban_Hang_Le.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning_Code\Do_An_Tot_Nghiep\Kinh_Doanh_Khoa_Hoc_Truc_Tuyen\Kinh_Doanh_Khoa_Hoc_Truc_Tuyen_Api\wwwroot\attachments\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456AA474-7DFC-4CE0-9BEA-D2FE68B000C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91138364-67F5-4E31-BA60-11D3A9015488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,13 +68,13 @@
     <t xml:space="preserve">Thành tiền (viết bằng chữ): </t>
   </si>
   <si>
-    <t xml:space="preserve">Email: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Người lập đơn: </t>
   </si>
   <si>
     <t>Mã Kích Hoạt</t>
+  </si>
+  <si>
+    <t>Email:</t>
   </si>
 </sst>
 </file>
@@ -264,8 +264,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -273,38 +300,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -637,40 +637,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+        <v>15</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -678,42 +678,42 @@
       <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+        <v>17</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+        <v>13</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+        <v>12</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -724,7 +724,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>10</v>
@@ -816,41 +816,48 @@
       <c r="E22"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:5" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="25" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="25"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="20" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="C8:D8"/>
@@ -863,13 +870,6 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.55069444444444449" right="0.2361111111111111" top="0.47222222222222221" bottom="0.35416666666666669" header="0.31458333333333333" footer="0.27500000000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>